<commit_message>
Divided CSS file into multiple files
</commit_message>
<xml_diff>
--- a/Dukementasjon/Dokumentasjon-plannlegging/Års-oppgave_plannlegging.xlsx
+++ b/Dukementasjon/Dokumentasjon-plannlegging/Års-oppgave_plannlegging.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udeoslokommuneno-my.sharepoint.com/personal/moaba161_osloskolen_no/Documents/KUBEN IT 23-24/IT/Års__Oppgave_Mohmed_IMA/Dukementasjon/Dokumentasjon-plannlegging/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udeoslokommuneno-my.sharepoint.com/personal/moaba161_osloskolen_no/Documents/KUBEN IT 23-24/IT/Års__Oppgave_Mohmed_IMA/Nettsiden/Dukementasjon/Dokumentasjon-plannlegging/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{E1382C03-4C16-4DCE-9B93-C8C8A6B04E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB2CC5A2-7850-40E2-BE93-292BB13B7538}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{E1382C03-4C16-4DCE-9B93-C8C8A6B04E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9388803E-983E-4481-94F1-1DC37E67B969}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{4969D71F-14DB-492F-97A2-90B2B97D0969}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="49">
   <si>
     <t>Dato</t>
   </si>
@@ -171,6 +171,18 @@
   </si>
   <si>
     <t>Ryddet og skjekke at alt er i orden</t>
+  </si>
+  <si>
+    <t>Uke 23</t>
+  </si>
+  <si>
+    <t>Forbedre oppgaven etter tilbakemeldningen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Oppløsning på bilder</t>
+  </si>
+  <si>
+    <t>Forminke CSS filen</t>
   </si>
 </sst>
 </file>
@@ -592,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4352DFF-A223-4A56-A395-F4AB5C385636}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="A1:K29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1103,6 +1115,31 @@
         <v>14</v>
       </c>
     </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>